<commit_message>
updating catalysis processes classes, attributes missing
</commit_message>
<xml_diff>
--- a/project/excel/hzb_catalysislabs_schema.xlsx
+++ b/project/excel/hzb_catalysislabs_schema.xlsx
@@ -23,24 +23,37 @@
     <sheet name="Mixture" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Workflow" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Process" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Experiment" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Measurement" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Parameter" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Reaction" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="ReactionProduct" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Reactor" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="CatalysisSampleCollection" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="ReactionProductCollection" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Beamline" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="BeamlineExperiment" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="BeamlineScientist" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="mySpot" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="EMIL_Pink" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="EMIL_OAESE" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="SampleEnvironment" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="EnvironmentDynamics" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="SamplePositioning" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="File" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="SynthesisProcess" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="CleaningProcess" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="CharacterizationProcess" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="CatalyticActivityAssesmentProcess" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="AnalyticsProcess" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="OzoneCleaning" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="CVD" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="CVD_nanofab" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CVD_pc1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CVD_pc2" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="sputtering" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="sputtering_prevac" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="sputtering_vonAdenne" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Experiment" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Measurement" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Parameter" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Reaction" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="ReactionProduct" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="Reactor" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CatalysisSampleCollection" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="ReactionProductCollection" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="Beamline" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="BeamlineExperiment" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="BeamlineScientist" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="mySpot" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="EMIL_Pink" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="EMIL_OAESE" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="SampleEnvironment" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="EnvironmentDynamics" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SamplePositioning" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="File" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1319,82 +1332,245 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>experiment_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>experiment_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>performed_by</t>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>identifierType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>creators</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>related_project</t>
+          <t>title</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>catalyst</t>
+          <t>Publisher</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sample</t>
+          <t>ResourceType</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>reaction</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>start_date</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>end_date</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>AlternateIdentifier</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>iri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>RelatedIdentifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Size</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Format</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Rights</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>GeoLocation</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>FundingReference</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>RelatedItem</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1430,7 +1606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1466,143 +1642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:W1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>identifierType</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>creators</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Publisher</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>ResourceType</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Subject</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Contributor</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Language</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>AlternateIdentifier</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>RelatedIdentifier</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Format</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Rights</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>GeoLocation</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>FundingReference</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>RelatedItem</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>iri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1638,7 +1678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1674,7 +1714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1710,58 +1750,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1804,71 +1792,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>experiment_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>experiment_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>performed_by</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>related_project</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>catalyst</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>reaction</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>start_date</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>end_date</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -1880,6 +1823,114 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2000,7 +2051,88 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>experiment_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>performed_by</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>related_project</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>catalyst</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>reaction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2036,7 +2168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2072,7 +2204,380 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>experiment_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>experiment_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>performed_by</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>related_project</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>catalyst</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>reaction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>project_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>project_code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>acronym</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>institutions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>principal_investigator</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>assigned_lab</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>research_area</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>collaborators</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2193,7 +2698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2229,7 +2734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2265,7 +2770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2301,7 +2806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2337,7 +2842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2373,92 +2878,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>project_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>project_code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>acronym</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>start_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>end_date</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>institutions</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>principal_investigator</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>assigned_lab</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>research_area</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>collaborators</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>

</xml_diff>

<commit_message>
adding sputtering prevac attributes
</commit_message>
<xml_diff>
--- a/project/excel/hzb_catalysislabs_schema.xlsx
+++ b/project/excel/hzb_catalysislabs_schema.xlsx
@@ -29,31 +29,33 @@
     <sheet name="CatalyticActivityAssesmentProcess" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="AnalyticsProcess" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="OzoneCleaning" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="CVD" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="CVD_nanofab" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CVD_pc1" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="CVD_pc2" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="sputtering" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="sputtering_prevac" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="sputtering_vonAdenne" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="Experiment" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="Measurement" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="Parameter" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="Reaction" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="ReactionProduct" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="Reactor" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CatalysisSampleCollection" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="ReactionProductCollection" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="Beamline" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="BeamlineExperiment" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="BeamlineScientist" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="mySpot" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="EMIL_Pink" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="EMIL_OAESE" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="SampleEnvironment" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="EnvironmentDynamics" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="SamplePositioning" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="File" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="ALD" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="ALD_BeneQ" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="CVD" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="CVD_nanofab" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CVD_pc1" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CVD_pc2" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Sputtering" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Sputtering_prevac" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="sputtering_vonAdenne" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Experiment" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Measurement" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Parameter" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="Reaction" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="ReactionProduct" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="Reactor" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="CatalysisSampleCollection" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="ReactionProductCollection" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="Beamline" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="BeamlineExperiment" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="BeamlineScientist" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="mySpot" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="EMIL_Pink" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="EMIL_OAESE" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SampleEnvironment" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="EnvironmentDynamics" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="SamplePositioning" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="File" sheetId="49" state="visible" r:id="rId49"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2057,6 +2059,183 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sputtering_prevac_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>substrate_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sample_owner</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>process_user</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>step_number</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>orientation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>sputter_pressure</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>substrate_temperature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>rotation</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>z_position</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>gas</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>flow_rate</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>target_position</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>target_power</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>DC_RF</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2132,7 +2311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2168,7 +2347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2204,7 +2383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2240,7 +2419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2276,7 +2455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2312,7 +2491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2338,7 +2517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2364,7 +2543,103 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>project_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>project_code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>acronym</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>institutions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>principal_investigator</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>assigned_lab</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>research_area</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>collaborators</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2400,7 +2675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2481,103 +2756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>project_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>project_code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>acronym</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>start_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>end_date</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>institutions</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>principal_investigator</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>assigned_lab</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>research_area</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>collaborators</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>iri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2698,7 +2877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2734,7 +2913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2770,7 +2949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2806,7 +2985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2842,7 +3021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2878,7 +3057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2914,7 +3093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>